<commit_message>
Add feature, edit UI, delete UI
</commit_message>
<xml_diff>
--- a/data/stocks.xlsx
+++ b/data/stocks.xlsx
@@ -16,7 +16,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -28,6 +28,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <color rgb="FF000000"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="1"/>
       <sz val="11"/>
     </font>
   </fonts>
@@ -58,7 +64,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
@@ -68,6 +74,15 @@
     </xf>
     <xf numFmtId="7" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="7" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
@@ -446,7 +461,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,10 +469,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="4" min="1" max="1"/>
-    <col width="18.71928571428571" bestFit="1" customWidth="1" style="5" min="2" max="2"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="6" min="3" max="3"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="4" max="4"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="1" max="1"/>
+    <col width="18.71928571428571" bestFit="1" customWidth="1" style="8" min="2" max="2"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="9" min="3" max="3"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="10" min="4" max="4"/>
   </cols>
   <sheetData>
     <row r="1" ht="19.5" customHeight="1">
@@ -466,7 +481,7 @@
           <t>Index</t>
         </is>
       </c>
-      <c r="B1" s="5" t="inlineStr">
+      <c r="B1" s="8" t="inlineStr">
         <is>
           <t>Product Name</t>
         </is>
@@ -486,7 +501,7 @@
       <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="inlineStr">
+      <c r="B2" s="8" t="inlineStr">
         <is>
           <t>Men's T-Shirt</t>
         </is>
@@ -502,7 +517,7 @@
       <c r="A3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="5" t="inlineStr">
+      <c r="B3" s="8" t="inlineStr">
         <is>
           <t>Women's Blouse</t>
         </is>
@@ -518,7 +533,7 @@
       <c r="A4" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="5" t="inlineStr">
+      <c r="B4" s="8" t="inlineStr">
         <is>
           <t>Men's Jeans</t>
         </is>
@@ -534,7 +549,7 @@
       <c r="A5" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="5" t="inlineStr">
+      <c r="B5" s="8" t="inlineStr">
         <is>
           <t>Women's Dress</t>
         </is>
@@ -550,7 +565,7 @@
       <c r="A6" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="5" t="inlineStr">
+      <c r="B6" s="8" t="inlineStr">
         <is>
           <t>Kid's T-Shirt</t>
         </is>
@@ -566,7 +581,7 @@
       <c r="A7" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="5" t="inlineStr">
+      <c r="B7" s="8" t="inlineStr">
         <is>
           <t>Men's Shorts</t>
         </is>
@@ -582,7 +597,7 @@
       <c r="A8" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="5" t="inlineStr">
+      <c r="B8" s="8" t="inlineStr">
         <is>
           <t>Women's Skirt</t>
         </is>
@@ -598,7 +613,7 @@
       <c r="A9" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="5" t="inlineStr">
+      <c r="B9" s="8" t="inlineStr">
         <is>
           <t>Men's Hoodie</t>
         </is>
@@ -614,7 +629,7 @@
       <c r="A10" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="5" t="inlineStr">
+      <c r="B10" s="8" t="inlineStr">
         <is>
           <t>Women's Sweater</t>
         </is>
@@ -630,7 +645,7 @@
       <c r="A11" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B11" s="5" t="inlineStr">
+      <c r="B11" s="8" t="inlineStr">
         <is>
           <t>Kid's Jeans</t>
         </is>
@@ -646,7 +661,7 @@
       <c r="A12" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="B12" s="5" t="inlineStr">
+      <c r="B12" s="8" t="inlineStr">
         <is>
           <t>Men's Sneakers</t>
         </is>
@@ -662,7 +677,7 @@
       <c r="A13" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="B13" s="5" t="inlineStr">
+      <c r="B13" s="8" t="inlineStr">
         <is>
           <t>Women's Sandals</t>
         </is>
@@ -678,7 +693,7 @@
       <c r="A14" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="B14" s="5" t="inlineStr">
+      <c r="B14" s="8" t="inlineStr">
         <is>
           <t>Kid's Sneakers</t>
         </is>
@@ -694,7 +709,7 @@
       <c r="A15" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="B15" s="5" t="inlineStr">
+      <c r="B15" s="8" t="inlineStr">
         <is>
           <t>Men's Belt</t>
         </is>
@@ -710,7 +725,7 @@
       <c r="A16" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="B16" s="5" t="inlineStr">
+      <c r="B16" s="8" t="inlineStr">
         <is>
           <t>Women's Handbag</t>
         </is>
@@ -722,23 +737,75 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" t="n">
+    <row r="17" ht="19.5" customHeight="1">
+      <c r="A17" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="B17" t="inlineStr">
+      <c r="B17" s="8" t="inlineStr">
         <is>
           <t>cargo</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>500</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>10</t>
+      <c r="C17" s="3" t="n">
+        <v>500</v>
+      </c>
+      <c r="D17" s="1" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" ht="18.75" customHeight="1">
+      <c r="A18" s="4" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="8" t="inlineStr">
+        <is>
+          <t>Saree</t>
+        </is>
+      </c>
+      <c r="C18" s="9" t="n">
+        <v>1234</v>
+      </c>
+      <c r="D18" s="10" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>saree</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>1111</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>222</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Shirt</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>34</t>
         </is>
       </c>
     </row>

</xml_diff>